<commit_message>
add SMIB modify by adding 1 gen to Bus1
</commit_message>
<xml_diff>
--- a/andes/cases/smib/SMIB.xlsx
+++ b/andes/cases/smib/SMIB.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cuiha\Dropbox\notebooks\tmp\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{254FE769-EF03-47A6-8662-B9BAC2A599B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="33090" yWindow="8085" windowWidth="16470" windowHeight="9090" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="20490" windowHeight="7635"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="9" r:id="rId1"/>
@@ -23,12 +17,54 @@
     <sheet name="Area" sheetId="7" r:id="rId8"/>
     <sheet name="GENCLS" sheetId="8" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="89">
+  <si>
+    <t>uid</t>
+  </si>
+  <si>
+    <t>field</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>comment2</t>
+  </si>
+  <si>
+    <t>comment3</t>
+  </si>
+  <si>
+    <t>comment4</t>
+  </si>
+  <si>
+    <t>Credit</t>
+  </si>
+  <si>
+    <t>This case is created by Xiaoge Huang based on the book "Power System Dynamics and Stability" by Sauer, Pai and Chow</t>
+  </si>
+  <si>
+    <t>Edits</t>
+  </si>
+  <si>
+    <t>Ths case is modified by Hantao Cui to use a base of 100 MVA to produce the same per-unit result as in the book</t>
+  </si>
+  <si>
+    <t>How</t>
+  </si>
+  <si>
+    <t>Essentially, the power base of all devices are converted to 100 MVA.</t>
+  </si>
+  <si>
+    <t>link</t>
+  </si>
+  <si>
+    <t>https://courses.physics.illinois.edu/ece576/sp2018/Sauer%20and%20Pai%20book%20-%20Jan%202007.pdf</t>
+  </si>
   <si>
     <t>idx</t>
   </si>
@@ -54,9 +90,6 @@
     <t>rf</t>
   </si>
   <si>
-    <t>uid</t>
-  </si>
-  <si>
     <t>Fault_1</t>
   </si>
   <si>
@@ -189,18 +222,18 @@
     <t>Line_1</t>
   </si>
   <si>
+    <t>Line 1</t>
+  </si>
+  <si>
     <t>Line_2</t>
   </si>
   <si>
+    <t>Line 2</t>
+  </si>
+  <si>
     <t>Line_3</t>
   </si>
   <si>
-    <t>Line 1</t>
-  </si>
-  <si>
-    <t>Line 2</t>
-  </si>
-  <si>
     <t>Line 3</t>
   </si>
   <si>
@@ -249,58 +282,31 @@
     <t>GENCLS_1</t>
   </si>
   <si>
+    <t>GENCLS 1</t>
+  </si>
+  <si>
     <t>GENCLS_2</t>
   </si>
   <si>
-    <t>GENCLS 1</t>
-  </si>
-  <si>
     <t>GENCLS 2</t>
-  </si>
-  <si>
-    <t>field</t>
-  </si>
-  <si>
-    <t>comment</t>
-  </si>
-  <si>
-    <t>comment2</t>
-  </si>
-  <si>
-    <t>comment3</t>
-  </si>
-  <si>
-    <t>comment4</t>
-  </si>
-  <si>
-    <t>Credit</t>
-  </si>
-  <si>
-    <t>This case is created by Xiaoge Huang based on the book "Power System Dynamics and Stability" by Sauer, Pai and Chow</t>
-  </si>
-  <si>
-    <t>Edits</t>
-  </si>
-  <si>
-    <t>Ths case is modified by Hantao Cui to use a base of 100 MVA to produce the same per-unit result as in the book</t>
-  </si>
-  <si>
-    <t>How</t>
-  </si>
-  <si>
-    <t>Essentially, the power base of all devices are converted to 100 MVA.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -308,19 +314,356 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -343,9 +686,251 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -353,20 +938,111 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
+    <cellStyle name="Title" xfId="39" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
+    <cellStyle name="Comma" xfId="44" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
+    <cellStyle name="Percent" xfId="47" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1314450" y="1285875"/>
+          <a:ext cx="4419600" cy="1657350"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -412,7 +1088,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -445,26 +1121,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -497,23 +1156,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -684,122 +1326,135 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:F4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="5"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="2:3">
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3">
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>80</v>
+      <c r="C3" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C2" t="s">
-        <v>82</v>
+    <row r="4" spans="2:3">
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>85</v>
-      </c>
-      <c r="C4" t="s">
-        <v>86</v>
+    <row r="5" spans="2:3">
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="E2">
         <v>3</v>
@@ -811,7 +1466,7 @@
         <v>0.2</v>
       </c>
       <c r="H2">
-        <v>1E-4</v>
+        <v>0.0001</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -819,65 +1474,68 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="3"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -921,7 +1579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -965,7 +1623,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1011,67 +1669,70 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="E2">
         <v>3</v>
@@ -1097,91 +1758,94 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="R1" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="E2">
         <v>100</v>
@@ -1220,7 +1884,7 @@
         <v>0.5</v>
       </c>
       <c r="R2">
-        <v>1E-8</v>
+        <v>1e-8</v>
       </c>
       <c r="S2">
         <v>0.3</v>
@@ -1228,94 +1892,97 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="L1" s="1" t="s">
+      <c r="R1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>14</v>
-      </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="E2">
         <v>100</v>
@@ -1354,7 +2021,7 @@
         <v>0.5</v>
       </c>
       <c r="R2">
-        <v>1E-8</v>
+        <v>1e-8</v>
       </c>
       <c r="S2">
         <v>0.3</v>
@@ -1365,106 +2032,109 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:X4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="3"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -1518,18 +2188,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -1583,18 +2253,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -1650,35 +2320,38 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1689,111 +2362,114 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:V3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="2"/>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="I2">
         <v>100</v>
@@ -1808,10 +2484,10 @@
         <v>1</v>
       </c>
       <c r="M2">
-        <v>5.7511999999999999</v>
+        <v>5.7512</v>
       </c>
       <c r="N2">
-        <v>1E-8</v>
+        <v>1e-8</v>
       </c>
       <c r="O2">
         <v>0.15</v>
@@ -1838,24 +2514,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="E3">
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="I3">
         <v>1000000000</v>
@@ -1873,10 +2549,10 @@
         <v>6</v>
       </c>
       <c r="N3">
-        <v>1E-8</v>
+        <v>1e-8</v>
       </c>
       <c r="O3">
-        <v>1E-8</v>
+        <v>1e-8</v>
       </c>
       <c r="P3">
         <v>0.01</v>
@@ -1902,5 +2578,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>